<commit_message>
update script with chromedriver_autoinstaller to avoid downloading Chromedriver and version issue
</commit_message>
<xml_diff>
--- a/static/excel/df_query.xlsx
+++ b/static/excel/df_query.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,21 @@
           <t>url_query</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>établissement co-accrédité</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>établissement délivrant conjointement le doctorat</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>établissement de préparation de la thèse</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -646,6 +661,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -753,6 +783,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -860,6 +905,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -967,6 +1027,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1074,6 +1149,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1181,6 +1271,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1288,6 +1393,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1395,6 +1515,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1502,6 +1637,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1609,6 +1759,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1716,6 +1881,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1823,6 +2003,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1930,6 +2125,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2037,6 +2247,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2144,6 +2369,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2251,6 +2491,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2358,6 +2613,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2465,6 +2735,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2572,6 +2857,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2679,6 +2979,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2786,6 +3101,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2893,6 +3223,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3000,6 +3345,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3107,6 +3467,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3214,6 +3589,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3321,6 +3711,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3428,6 +3833,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3535,6 +3955,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3642,6 +4077,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3749,6 +4199,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3856,6 +4321,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3963,6 +4443,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4070,6 +4565,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4177,6 +4687,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4284,6 +4809,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4391,6 +4931,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4498,6 +5053,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4605,6 +5175,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4712,6 +5297,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4819,6 +5419,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4926,6 +5541,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5033,6 +5663,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5140,6 +5785,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5247,6 +5907,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5354,6 +6029,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5461,6 +6151,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5569,6 +6274,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5676,6 +6396,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5783,6 +6518,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5890,6 +6640,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5997,6 +6762,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -6104,6 +6884,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6211,6 +7006,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6318,6 +7128,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6425,6 +7250,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6532,6 +7372,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6639,6 +7494,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6746,6 +7616,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6853,6 +7738,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6960,6 +7860,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -7067,6 +7982,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -7174,6 +8104,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -7281,6 +8226,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7388,6 +8348,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7495,6 +8470,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7602,6 +8592,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7709,6 +8714,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7816,6 +8836,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7923,6 +8958,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -8030,6 +9080,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -8137,6 +9202,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -8244,6 +9324,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -8351,6 +9446,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -8458,6 +9568,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -8565,6 +9690,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -8672,6 +9812,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -8779,6 +9934,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -8886,6 +10056,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8993,6 +10178,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V80" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -9100,6 +10300,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W81" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -9207,6 +10422,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -9314,6 +10544,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -9421,6 +10666,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V84" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W84" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -9468,7 +10728,11 @@
           <t>Cette thèse traite de la dynamique des filaments d’upwelling. Trois mécanismes de formation sont étudiés au travers de deux études de processus et de données in-situ et télédétectées. L’impact de la topographie de fond sur la génération et le piégeage de filaments sont étudiés à l’aide d’un modèle shallow water à deux couches. Il est montré que la génération d’anomalie de vorticité potentielle piégée au dessus d’un promontoire induit une circulation permanente qui pince le front et l’entraîne loin au large. La sensibilité du processus à de nombreux paramètres est étudIée. L'interaction entre un jet de surface et un courant profond séparés par une couche intermédiaire sans anomalie de PV est également étudiée à l’aide d’un modèle shallow water. Une analyse de stabilité linéaire montre que ce système de courant est instable barocliniquement et qu’il existe toujours une longueur d’onde instable quelle que soit l’épaisseur de la couche intermédiaire. Il est montré que l’interaction entre des structures vorticales profondes et un front de surface stable peut générer des méandres et des filaments. Enfin, la dynamique des filaments d’upwelling au large de Cap Blanc (Mauritanie) est étudiée à l’aide de données in-situ et télédétectées. La présence de tourbillons issus du front du Cap Vert joue un rôle clé dans la formation des filaments. La topographie semble également jouer un rôle important, avec la formation d’un anticyclone au dessus d’un large promontoire. De manière générale, il est montré que les filaments d’upwelling résultent de l’interaction de structures vorticales et d’un front côtier.</t>
         </is>
       </c>
-      <c r="J85" t="inlineStr"/>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
       <c r="K85" t="inlineStr">
         <is>
           <t>Missing Value</t>
@@ -9522,6 +10786,21 @@
       <c r="U85" t="inlineStr">
         <is>
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V85" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W85" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>Missing value</t>
         </is>
       </c>
     </row>
@@ -9631,6 +10910,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W86" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -9738,6 +11032,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V87" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W87" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -9845,6 +11154,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V88" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -9952,6 +11276,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V89" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W89" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -10059,6 +11398,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V90" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W90" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -10166,6 +11520,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V91" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -10273,6 +11642,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V92" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W92" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -10380,6 +11764,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V93" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -10487,6 +11886,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V94" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -10594,6 +12008,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V95" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -10701,6 +12130,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V96" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -10808,6 +12252,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W97" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -10915,6 +12374,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V98" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W98" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -11022,6 +12496,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V99" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -11129,6 +12618,21 @@
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
         </is>
       </c>
+      <c r="V100" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X100" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -11234,6 +12738,1612 @@
       <c r="U101" t="inlineStr">
         <is>
           <t>https://theses.fr/resultats?q=water&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V101" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Jean-Charles Moretti</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  René Ginouvès</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Arts du spectacle</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance en 1989</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Paris 10</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Le théâtre d’Argos est situé au pied du promontoire que présente l'acropole de la cite, la Larissa, à l'extrémité sud de son flanc est. Le premier état de l'édifice date du premier quart du IIIe siècle avant J. -C. Son bâtiment de skènè comportait un prosternions, probablement ionique, une skènè de plan rectangulaire dotée d'un front de scène perce de cinq larges baies, deux rampes conduisant à l'étage de la skènè et à l'estrade du proskenion et un portique dorique adossé à la skènè. Un cercle de dalles de calcaire, côtoyé de deux tangentes, était inscrit dans l'orchestra, à laquelle on pouvait accéder, de la scène, par un passage souterrain. Le koilon, dont les kerkis centrales étaient taillées dans le rocher et les kerkis latérales construites, avait une capacité de vingt mille places. A l'époque d'Hadrien, vraisemblablement aux frais de l'empereur, l'édifice scénique fut remodelé. Il fut doté d'un pulpitum bas et profond, côtoyé de deux parascaenia, et d'une frons scaenae rectiligne percée de trois portes. Le théâtre, où se déroula dès le troisième siècle avant J. -C. La partie musicale et dramatique des concours nemeens, accueillit, a l'époque impériale, dans son orchestra, des chasses, des combats de gladiateurs et des thetymimes.</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>Le théâtre d'Argos</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>https://theses.fr/1989PA100091</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>Le théâtre d’Argos est situé au pied du promontoire que ... orchestra, des chasses, des combats de gladiateurs et des thetymimes.</t>
+        </is>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Camille Prieur</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Francesca Prescendi morresi, Véronique Dasen</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Projet de thèse</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Histoire des religions et anthropologie religieuse</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Inscription en doctorat le 31/05/2023</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Université Paris sciences et lettres en cotutelle avec Université de Fribourg</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale de l'École pratique des hautes études (Paris)</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Ce projet de thèse a pour but d'étudier l'ensemble des protections religieuses et symboliques utilisées par les hommes dont la vie et l'honneur sont en danger dans les contextes de guerre, des combats, compétitions et spectacles armés et non armés durant l'Empire Romain (Ier siècle av. J-C  IVème siècle apr. J-C). Ce travail offrira un nouvel angle d'étude aux multiples recherches qui depuis une dizaine d'année s'intéressent aux risques ainsi qu'aux moyens de protections dédiées aux femmes et aux enfants. Cette recherche ne traitera pas de ces derniers mais proposera une nouvelle approche sur les hommes « à risques ». Contrairement aux études existantes aujourd'hui ne se centrant que sur une catégorie d'homme à risques, ce projet mettra en avant une nouvelle approche globale de ces individus, de leurs religions personnelles et de son expression matériel et immatérielle (artéfacts, gestes+). L'objectif de ce projet est d'analyser les divers moyens utilisés par les empereurs, soldats, marins, gladiateurs, conducteurs de char, musiciens, acteurs et acrobates, dans des situations où ils mettent leur vie ou leur honneur en danger, cherchant à obtenir une protection supplémentaire conférée par les dieux afin d'assurer le succès, de se protéger des coups du sort ou de leur adversaire, des blessures et de la mort. Pour réaliser ce projet et répondre à l'ensemble des problématique posées, nous nous intéresserons à l'étude des amulettes, gemmes, équipements/armements, tablettes de malédictions, sans négliger l'ornementation corporelle (tatouages). Cette thèse a pour objectif de contribuer au renouvellement du regard porté sur les notions de masculinité et de risque dans le monde romain. Nous nous intéresserons également aux traces des différentes croyances et pratiques religieuses manifestées dans un contexte privé et publics, par des gestes et surtout l'utilisation d'artéfacts de natures variées. Ce projet contribuera à la construction d'une histoire de la religion vécue dans ses différentes expressions, en mettant en lumière d'une part en quoi consistent leurs besoins de protection, d'autre part les ressources mobilisées pour faire face aux dangers. Notre démarche croisera donc trois approches méthodologiques, propre à l'étude du matériel archéologique, l'histoire des religions ainsi que l'iconographie. Ce travail repose sur le dépouillement d'ouvrages, de catalogue et de bases de données ; la création d'un catalogue et d'une base de données propre au projet, le traitement d'image (graphique et numérique). Ce projet appliquera à chaque catégorie de sources les méthodes d'analyse de la discipline : mise en contexte des textes et des artéfacts, mise en série des objets et des images. Cette recherche sera aussi menée de manière transdisciplinaire et comparatiste, en s'intéressant aux moyens de protection des combattants dans le monde grec ainsi qu'au Moyen âge et à la Renaissance.</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>Les hommes à risques dans le monde romain. Études des objets « protecteurs » et de leur symbolique</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>https://theses.fr/s369831</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EPHE PARIS</t>
+        </is>
+      </c>
+      <c r="T103" t="inlineStr">
+        <is>
+          <t>Ce projet de thèse a pour but d'étudier l'ensemble des ... monde grec ainsi qu'au Moyen âge et à la Renaissance.</t>
+        </is>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X103" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Jérôme Kennedy</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Stéphane Benoist</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Histoire romaine</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance le 22/06/2019</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Université de Lille (2018-2021)</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale Sciences de l'homme et de la société (Lille ; 2006-....)</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Quiconque a déjà vu Gladiator de Ridley Scott a pu observer Joaquin Phoenix incarner un bien cruel empereur Commode, maître des armes et détenteur d’un pouvoir absolu, qui, isolé dans son palais, peut décider de la vie et de la mort de ses sujets. Mais il a également pu voir Derek Jacobi jouer le sénateur Gracchus, farouche partisan de la res publica (notion qui, dans ce contexte, prend le sens de République), système politique qui existait avant que ne soit créé le pouvoir des empereurs. Ce clivage politique entre pouvoir personnel et exercice collégial du gouvernement ne correspond en rien à la réalité historique propre à l’époque du dernier des Antonins, mais il est assurément le reflet de ce que l’imaginaire commun a pu retenir de cette période de l’Antiquité. Cette approche duale et contradictoire du pouvoir politique romain n’est pas une invention des Modernes. Elle peut renvoyer, certes de manière très schématique, à la période qui, du Ier siècle avant notre ère au Ier siècle de notre ère, voit émerger non pas un changement de régime mais un entre-deux politique, entre démocratie et monarchie, où le pouvoir impérial fondé par Auguste au tournant de notre ère fait sienne toute une culture nobiliaire du pouvoir tout en développant un contact et une réelle interaction avec le populus de Rome et, plus largement les habitants de l’imperium Romanum. C’est à cela même que renvoie la notion de « République impériale » romaine. Le recours à ce concept peut paraître surprenant puisqu’il a surtout été utilisé par des historiens de l’époque contemporaine, que l’on songe à Raymond Aron ou Olivier Le cour Grandmaison mais il permet de rendre compte des nuances propres à cette période où, pour paraphraser le philosophe Cicéron, des individus ont bénéficié « d’un pouvoir supérieur à celui de l’État tout entier » sans pour autant que les structures de celui-ci ne soient brutalement remises en cause. Complexe à définir et tout à fait spécifique, cet entre-deux ne peut être compris que dans une dynamique de mutation, ses structures militaires, économiques, politiques et, pour reprendre un terme actuel bien qu’inadapté, idéologiques évoluant à mesure que se renforce l’administration du « monde romain » - qui s’étend sur une partie de l’Europe, de l’Asie et de l’Afrique - mais aussi que les habitants de cet ensemble ne s’habituent au pouvoir personnel. En prenant appui sur les acquis récents de l’historiographie tout autant que sur les controverses qui lui sont propres (citons à titre d’exemple l’opposition de vue entre Fergus Millar et Karl-Joachim Hölkeskamp à propos de la nature démocratique et/ou aristocratique de la res publica romaine), la présente enquête entend renouveler la perception de cadres chronologiques souvent réduits à une succession République/Empire afin de percevoir au mieux les modalités d’enracinement d’un pouvoir personnel et centralisé au sein d’un « monde romain », dont la capitale continue d’être pensée comme une cité où le pouvoir s’incarne aux travers de magistratures et de l’ordre sénatorial. Ancrée dans le champ politique et institutionnel, cette réflexion ne peut faire abstraction des apports qui sont ceux de la sociologie mais aussi de la science politique, y compris dans ses aspects les plus récents, afin de saisir comment un système politique peut profondément évoluer sans pour autant changer brutalement, soit un questionnement très actuel à l’heure où le modèle démocratique tel que forgé au sortir de la Seconde Guerre mondiale tend à être remis en cause.</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>Une "République impériale" en mutation : pensée politique, institutions et société romaine de l'époque de Sylla (138-78 av. n. è.) à la fin du Ier siècle de n. è.</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2019LILUH021</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Président / Présidente </t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Stéphane Benoist, Sylvie Pittia, Frédéric Hurlet, Harriet I. Flower</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sylvie Pittia, Frédéric Hurlet</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>Quiconque a déjà vu Gladiator de Ridley Scott a pu ... la Seconde Guerre mondiale tend à être remis en cause.</t>
+        </is>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Robin Delory</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Olivier Sirost</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Staps</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance le 15/12/2023</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Normandie</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale Homme, sociétés, risques, territoire (Rouen)</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Dans un paysage sportif marqué par la prolifération et l’intégration de nouvelles technologies (Thorpe, 2016), se développe une discipline singulière et controversée : le mixed martial arts (MMA). Agrégat de tous les arts martiaux, il fut dès son apparition présenté comme une transgression absolue des droits de l’homme renouant avec la mise à mort des gladiateurs des jeux du cirque. Bien que légal en France depuis 2020, il pose la logique contradictoire relevée par Norbert Elias : « l’un des problèmes essentiels concernant le sport, à savoir comment réconcilier deux fonctions contradictoires : d’une part, le relâchement agréable du contrôle exercé sur les sentiments humains, la manifestation d’une excitation agréable, et, d’autre part, le maintien d’un ensemble de codifications pour garder la maîtrise des émotions agréablement décontrôlées » (Elias, Dunning 1994). Le MMA partage plusieurs homologies avec le « jeu vidéo de combat » (JVC), autre objet régulièrement délégitimé pour son caractère violent.Notre étude se propose de penser l’émergence et le succès de ces disciplines en parallèle aux processus à l’œuvre de déclin du sport moderne et de développement d’autres formes de pratiques sportives (postmodernes). Il s’agit de plus, par approches comparatives, d’étudier leur mode de diffusion et la manière dont elles participent à la construction d’un nouvel imaginaire sportif fondé sur la mise en image de combattants et d’affrontements contribuant au développement de récits transmédia (Jenkins, 2009). Aussi, le travail consiste à examiner les modalités d’intégration et de représentations de la violence chez les pratiquants issus de ces deux univers.Pour ce faire, deux revues systématiques internationales (l’une sur le MMA, l’autre sur le jeu vidéo de combat (JVC)) ont été conduites, trois terrains ethnographiques – deux clubs de MMA et une association de jeu vidéo de combat – ont été étudiés et une enquête par questionnaires menée auprès de 500 pratiquants a été réalisée. L’étude traite transversalement des enjeux éthiques et déontologiques impliqués par les modalités d’engagement d’un chercheur enquêtant par corps ainsi qu’en terrain sensible et familier.Les résultats mettent en lumière la nature totalement incarnée du MMA et du jeu vidéo de combat, et révèlent accessoirement l’existence d’analogies dans les engagements sensoriels et émotionnels vécus à travers leur pratique. Par leurs spécificités, ces disciplines apparaissent également comme réponses à la quête de sens, de significations, d’identité et à la saturation caractéristique de la vie quotidienne. Ce travail montre en outre la manière dont la diffusion d’images de MMA au travers différents supports – dont le jeu vidéo de combat – participe à la construction et intégration d’un nouvel imaginaire sportif redéfinissant les modes de représentations et favorisant la circulation entre (voire transcendant) les frontières temporelles, géographiques et culturelles par hybridation des usages et pratiques médiatiques et sportives.</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>ΜΜA et JVC : ethnographie d'une transfiguration sportive</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2023NORMR101</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Président / Présidente </t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Judit Vari, Pascal Roland</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bernard Andrieu, Robin Recours</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T105" t="inlineStr">
+        <is>
+          <t>Dans un paysage sportif marqué par la prolifération et l’intégration ... culturelles par hybridation des usages et pratiques médiatiques et sportives.</t>
+        </is>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Université de Rouen Normandie (1966-....)</t>
+        </is>
+      </c>
+      <c r="W105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X105" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  André Tessier</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Emmanuel Désveaux</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Anthropologie sociale et ethnologie</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance le 11/12/2018</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Paris Sciences et Lettres (ComUE) en cotutelle avec 060918977</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale de l'École des hautes études en sciences sociales</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  établissement de préparation de la thèse </t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>L’objet d’étude et le domaine de rechercheComme le sacré, le jeu et le sport délimitent dans le monde profane un espace réservé que régentent une série de règles et rituels qui n'ont de sens et de valeur que par la croyance qui leur est attribuée. Le lieu sacré est l’Aréna, le Colisée ou le Forum. Espace plus restreint, la « chambre de hockey » est une sphère sacrée privée, où entrent uniquement les gens autorisés, ce que nous appelons le « Dernier bastion des mâles ». On pourrait l’appeler aussi le « quartier des hommes » maanabeu chez les Lau ou la « Maison des hommes » chez les Baruya en passant par la Californie et l’Amazonie, les « Maisons de sudation ». Sujets tabous, secrets, histoires grivoises et anecdotes sont échangées; c’est là que les confidences se font et que se tissent les liens. On réfèrera aux notions d’espace sportif de Bromberger (1996), de masculinité et de féminité de Saouter (2000) et du système sportif de Darbon (2014). Il y a plusieurs niveaux d’identités, particulièrement la création du sentiment d’appartenance et de la confrérie.Rituels et rite initiatique – La masculinité et la séductionPour maintenir l’ordre social de la chance et de la victoire, plusieurs types de rituels sont présents et dans certains cas servent même à profaner les chances de l’équipe adverse. Les joueurs ont ainsi recours à toute une gamme de rituels. Le monde des croyances sert à rendre le joueur invincible, à minimiser les blessures, à le propulser vers la victoire avec le but victorieux, à prendre la bonne décision et à sortir vainqueur après chaque rencontre. L’analyse structurale « revisitée » vient nous porter main forte afin de bien comprendre tout cet univers symbolique du hockey en appliquant la formule canonique au sport et au genre. « Le hockey au Québec, est comme une religion ». Le hockey senior est un prétexte pour comprendre les profondes transformations et les influences qui viennent de toutes parts et sont réappropriées à travers les emprunts culturels. Aux besoins par la culture sportive, en même temps que les pratiques sociales sont transversales (Warnier, 2008), ainsi le « diffusionnisme contemporain » sert à suivre ces emprunts culturels, qui souvent proviennent des autochtones. On peut voir l’équipe de hockey comme une « tribu » avec son chef et ses guerriers qui prennent tous les moyens afin de pouvoir affirmer qu’ils sont ou ont été les plus forts, les vainqueurs de la « Coupe » à un moment donné de leur histoire, et ce, devant des femmes qu’ils tentent de séduire. Dans les sports de contact physique comme le hockey sur glace On les surnomme souvent « Gladiateurs » quand on voit leurs équipements, et leurs bâtons. Le hockey est un monde d’homme où la masculinité et la virilité sont encore présentes. Anne Saouter pose la bonne question dans sa recherche sur le rugby : « Mais le rugby, sport de la virilité par excellence dans l’imagerie collective, n’exige-t-il pas obligatoirement un jeu de miroir pour valider cette virilité : le regard des femmes?</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>Sport et masculinité : le cas de la culture du hockey senior au Québec</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2018PSLEH170</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Président / Présidente </t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Frédéric B. Laugrand, Christian Bromberger, Gilles Havard, Anne Saouter, Frédéric Saumade</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T106" t="inlineStr">
+        <is>
+          <t>L’objet d’étude et le domaine de rechercheComme le sacré, le ... miroir pour valider cette virilité : le regard des femmes?</t>
+        </is>
+      </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X106" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Frédérique Lambert</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Antoine de Baecque</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Arts du spectacle </t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance le 05/11/2020</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Paris 10</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale Lettres, langues, spectacles (Nanterre, Hauts-de-Seine ; 2000-....)</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Gladiator (Ridley Scott, 2000) inaugure une renaissance du genre péplum, mêlant dans l’esthétique post-moderne, culture patrimoniale et production de type blockbuster, cinéma d’action et cinéphilie. Les renaissances cycliques de ce genre dans l’histoire du cinéma sont liées à des innovations techniques et à une scénarisation du genre. Ici, les effets visuels revisitent dans un premier temps les scènes épiques clé (batailles rangées, destructions, décors, foules) et introduisent de nouveaux motifs (souffle, explosions, destructions) en utilisant des techniques et technologies hybrides (peinture, archéologie, jeux vidéo). De 2009 à 2014, la 3-D confère un second souffle à ce néo genre (immersions, jaillissements). Le storytelling biblique et l’esthétique de série ou de sport You Tube constituent le troisième temps de cette renaissance. Ce péplum est traditionnellement un genre d’adaptation sujet au remake. Les études de littérature comparée apportent un éclairage sur ces pratiques de reprise, qu’elles attribuent à l’epos, dans lequel le néo péplum s’inscrit. La pratique du remake correspond alors à une pratique typique de l’épopée qui permet de penser la crise politique en gestation. Les néo péplums fonctionnent dès lors génériquement comme signes de la crise en cours. Ces reprises offrent une grille de lecture permettant de penser l’inédit du changement en cours. Le motif du souffle épique surexploité dans ces néo péplums devient dès lors signifiant. De fait, les données économiques et la chronologie des crises politiques et géo stratégiques traversées par les Etats-Unis, confirment la dimension communicationnelle de ce genre à destination d’une communauté interprétative désormais mondialisée. De fait, l’héroïsme véhiculé et réactualisé dans les mythologies super héroïques traduisent les enjeux individuels et collectifs de la crise mondiale : une « médiamorphose » numérique dont ces néo péplums sont le reflet par leur esthétique, syntaxe et idéologie.</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>Permanences et variations du souffle épique numérique dans le néo péplum Hollywoodien (2000-2018)</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2020PA100076</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Président / Présidente </t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Antoine de Baecque, Réjane Hamus-Vallée, Martin Barnier, Christel Taillibert, Fabien Boully, Gaspard Delon</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Réjane Hamus-Vallée, Martin Barnier</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T107" t="inlineStr">
+        <is>
+          <t>Gladiator (Ridley Scott, 2000) inaugure une renaissance du genre péplum, ... péplums sont le reflet par leur esthétique, syntaxe et idéologie.</t>
+        </is>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thomas Marlier</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  André Laronde</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Histoire et civilisation de l'Antiquité</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance en 2004</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Paris 4</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Quelle est la part de tradition grecque et d'innovation romaine dans l'architecture d'une ancienne cité grecque durant le Haut-Empire ? Le cas de Cyrène et des quatre autres cités de la région - Apollonia, Ptolémai͏̈s, Taucheira et Bérénikè - montre qu'hellénisme et romanité sont souvent conjoints : la grande majorité des édifices conservent des procédés de constructions grecs, mais une grande partie des bâtiments neufs ou restaurés à cette époque recouvrent des types romains, notamment les théâtres, les temples et les arcs monumentaux. Des types complètement neufs comme l'amphithéâtre ou la basilique apparaissent, et certains ensembles monumentaux adoptent une configuration romaine : le forum de Cyrène, par exemple, associe un quadriportique à un temple et une basilique. Ça n'est pas dans la situation politique, démographique, religieuse ou sociale qu'on trouvera des explications aux innovations romaines. Il apparaît que le conservatisme des façons de construire s'explique essentiellement par une inertie du savoir-faire où les artisans et architectes en Cyrénai͏̈que reproduisent simplement leurs habitudes en utilisant le système technique qu'ils connaissent déjà. L'innovation romaine semble ressortir soit à un simple phénomène de mode où les nouveaux types architecturaux sont imités " pour faire romain " sans que de nouveaux usages romains leur correspondent ; soit, plus rarement, à la diffusion d'usages romains où de nouveaux types d'édifices sont nécessaires : l'apparition de l'amphithéâtre, par exemple, s'explique par la diffusion des spectacles de chasse et de gladiateurs dans cette région.</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>Tradition grecque et innovation romaine dans l'architecture en Cyrénai͏̈que à l'époque impériale: les monuments publics</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2004PA040096</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>Quelle est la part de tradition grecque et d'innovation romaine ... des spectacles de chasse et de gladiateurs dans cette région.</t>
+        </is>
+      </c>
+      <c r="U108" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X108" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Tom Fournier</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Pascal Puech, Benjamin Lassagne</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Projet de thèse</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Physique de la Matière</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Inscription en doctorat le 01/10/2022</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Université de Toulouse (2023-....)</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  SDM - SCIENCES DE LA MATIERE - Toulouse</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Une thèse, à cheval entre le CEMES et le LPCNO et financée par l'ANR dans le cadre du projet GLADIATOR est disponible à Toulouse (France). Elle a pour objectif de réaliser par hydrogénation localisée des hétérostructures planaires carbone sp3/carbone sp2, en d'autres termes réaliser des hétérostructures graphane/graphène ou diamane/graphène bi-couche. Leurs propriétés fondamentales (nano-optique, électronique +) seront étudiées afin d'envisager leur utilisation dans des dispositifs à l'échelle micro et nano pour diverses applications (détection, RF, biologie+). Ce projet rassemble des équipes impliquées soit dans la théorie et les calculs, soit dans l'expérimentation (synthèse et conception et fabrication de dispositifs). La thèse se focalisera sur la partie expérimentale. La toute première démonstration d'une synthèse réussie de diamane a été faite par notre consortium en 2020 (voir références). Ceci ouvre de nouvelles perspectives pour créer des hétérostructures et des dispositifs avec de nouvelles propriétés passionnantes. Les compétences requises pour ce travail de thèse nécessitera à la fois une bonne connaissance de la physique du solide et une certaine dextérité pour l'expérimentation. La manipulation précise de films 2D, leur structuration par des procédés en salle blanche, la caractérisation structurale et chimique des interfaces carbone sp2/p3 et les mesures de transport à basse température (typiquement hélium) seront les principales tâches à mener. Plusieurs longs séjours outre-mer en République Dominicaine et au Canada pour visiter nos partenaires (spécialisé en hydrogénation, +) sont prévus. Des masques de natures diverses (résine, BN+) seront utilisés pour hydrognéer les zones de graphène localement et ainsi former des matériaux 2D hybrides inédits. Les motifs seront adaptés soit à la caractérisation fine des interfaces carbone sp2/sp3 soit pour des applications spécifiques. Pour caractériser les zones hydrogénées et les interfaces carbone sp2/sp3, des techniques de champ proche (microscopie à force atomique, microscopie à sonde de potentiel de surface Kelvin, spectroscopie Raman améliorée par la pointe et microscopie à force photo-induite) seront utilisées. Les mesures de transport seront réalisées sur des nanorubans de graphène entourés de diamane.</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Couche de graphène avec parties isolantes en diamane pour dispositifs 2D</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>https://theses.fr/s357247</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T109" t="inlineStr">
+        <is>
+          <t>Une thèse, à cheval entre le CEMES et le LPCNO ... seront réalisées sur des nanorubans de graphène entourés de diamane.</t>
+        </is>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Institut national des sciences appliquées (Toulouse ; 1961-....)</t>
+        </is>
+      </c>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Méryl Ducros</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Éric Perrin-Saminadayar</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  HISTOIRE spécialité Histoire ancienne</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance le 09/12/2017</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Montpellier 3</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale Langues, Littératures, Cultures, Civilisations (Montpellier ; 1991-....)</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Les combats de gladiateurs sont les spectacles les mieux documentés du monde romain. Depuis l'ouvrage de Louis Robert (Les gladiateurs dans l'Orient Grec, Paris, 1940), qui rassemble un corpus épigraphique et iconographique très intéressant, aucune nouvelle synthèse n'a été proposée sur les gladiateurs en Orient, alors que les découvertes ont été très nombreuses, notamment en ce qui concerne les stèles funéraires. Le but de cette thèse sera de mettre en avent cette nouvelle pratique sociale apparue en Orient avec la conquête romaine à travers un catalogue de sources exhaustifs partant des travaux déjà effectués par Louis Robert, étoffés des découvertes postérieures afin d’établir une étude complète du phénomène.</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Les gladiateurs dans l'Orient grec : particularismes locaux, environnement social et représentations</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2017MON30064</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Président / Présidente </t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sandrine Agusta-Boularot, Karine Karila-Cohen</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pantelī́s M. Nígdelīs</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>Les combats de gladiateurs sont les spectacles les mieux documentés ... des découvertes postérieures afin d’établir une étude complète du phénomène.</t>
+        </is>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Manon Castelle</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Chantal Grell, David Bourgarit</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Histoire, histoire de l'art et archéologie</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance le 31/03/2016</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Université Paris-Saclay (ComUE)</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale Sciences de l'Homme et de la société (Sceaux, Hauts-de-Seine ; 2015-2020)</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laboratoire </t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>A partir de la fin de l’Antiquité, les grands bronzessont peu à peu délaissés puis abandonnés. Il faudra attendre laseconde moitié du XVIème siècle pour voir réapparaître dans lepaysage artistique français, sous François Ier, de grandsensembles statuaires en bronze. Au coeur de ce phénomène, latechnique tient un rôle majeur et suscite plusieursinterrogations. D’abord, se pose pour cette période la questionde l’existence ou non d’une identité technique des bronzesfrançais. L’exécution d’une statue en bronze implique denombreuses étapes qui conduisent du modèle à saretranscription dans le métal. Peut-on reconnaître dans cesétapes et dans les manières de les aborder une certaine unitétechnique qui marquerait la seconde moitié du XVIème siècle,voire le début du XVIIème en France ? Inversement, remarqueton dès cette période de réintroduction différentes écolesregroupant certains sculpteurs, fondeurs, ateliers, voire liées àcertains chantiers particuliers ? Par ailleurs, la réapparition dessavoir-faire associés à la statuaire en bronze pose la questiondes origines. D’où viennent ces techniques soi-disant oubliées :d’autres centres européens, de pratiques de fonderie concernantd’autres types de production ?Dans ce travail de thèse, nous nous sommes attachés à apporterdes éléments de réponse à ces différentes interrogations. Pource faire, des études technologiques ont été menées sur troisgrands ensembles marquant cette période de renouveau dansl’art du bronze : les copies en bronze de marbres antiques parPrimatice, les Vertus du monument funéraire d’Henri II et deCatherine de Médicis, les Allégories du monument de coeurd’Anne de Montmorency.Pour compléter ce corpus, des éléments isolés ont été étudiés :la Diane chasseresse de Barthélémy Prieur, l’Apollon duBelvédère, le Gladiateur Borghèse et la Vénus Médicisattribués à Hubert le Sueur. L’objectif a été de tenter de révélerprocédés, matériaux et savoir-faire engagés, complétant ainsiles données fournies par les documents d’archives quiaccompagnent ces commandes prestigieuses. La stratégied’étude employée a bénéficié de l’expérience des travauxentrepris ces trente dernières années. Des développementsméthodologiques ont néanmoins été nécessaires pour compléterles possibilités offertes par l’étude technologique de la statuaireen bronze. Ces développements ont en particulier concerné lesnoyaux de fonderie, ces matériaux employés pour réaliser desstatues creuses. Les résultats obtenus montrent que lespremières décennies de réappropriation de la grande statuaireen bronze sont marquées par l’emploi d’un même procédé àl’épargné qui trouve racine dans les procédés employés auMoyen-âge pour la fonte de cloches ou de canons par exemple.Mais dés le XVIIème siècle, le monopole de ce procédé sembleêtre mis à mal, preuve sans doute d’une émancipation desfondeurs et d’une innovation constante. Parallèlement à cesphénomènes dont les conséquences marquent la fonte statuaireen général, les sculpteurs, les fondeurs, développent dans leursateliers des savoir-faire personnels et innovent au cas par cas,selon la nature des commandes qu’ils reçoivent.</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>Les techniques de fabrication de la grande statuaire en bronze 1540-1660 en France</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2016SACLV097</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Président / Présidente </t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> David Bourgarit</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Francesca G. Bewer, Paolo Piccardo</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T111" t="inlineStr">
+        <is>
+          <t>A partir de la fin de l’Antiquité, les grands bronzessont ... au cas par cas,selon la nature des commandes qu’ils reçoivent.</t>
+        </is>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W111" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Université de Versailles-Saint-Quentin-en-Yvelines (1991-....)</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Gaspard Delon</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Laurence Schifano, Jean-Loup Bourget</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Histoire de l'art</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance en 2011</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Paris 10</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  École doctorale Lettres, langues, spectacles (Nanterre, Hauts-de-Seine ; 2000-....)</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>La banalisation de la scène de bataille rangée dans le cinéma hollywoodien contemporain accompagne le redressement de l’épopée historique, convalescente depuis les années 1960 mais revivifiée par les succès de « Braveheart » puis « Gladiator », ainsi que le développement du film de fantasy dans le sillage de « The Lord of the Rings ». La production de cette scène de genre, circonscrite mais remarquablement régulière entre 1999 et 2011, participe de la stratégie commerciale du blockbuster en visant un public large et international, et donne lieu à de nombreuses imitations dans les sphères voisines du paysage médiatique. Œuvre collective, elle combine savoir-faire technique traditionnel et recours croissant aux sociétés d’effets visuels, qui en font un terrain d’expérimentation privilégié et l’objet d’une lutte concurrentielle. La représentation des combats, qui tente de s’inscrire dans une prestigieuse tradition historique et artistique tout en se conformant aux normes du film d’action, s’appuie sur des stéréotypes formels et narratifs à l’origine d’un jeu de surenchère et de variation typique des mécanismes du formatage et de l’invention hollywoodiens. Entremêlant le récit et le spectaculaire, la scène de bataille est porteuse, pour le spectateur, de plaisirs et de sensations spécifiques. Limitée par l’ampleur et le réalisme des combats, l’héroïsation individuelle s’y articule avec une représentation de la collectivité en action et une mise à l’épreuve des certitudes bellicistes. Présumées routinières, répétitives, académiques ou idéologiquement conservatrices, les scènes de bataille rangée se révèlent ainsi porteuses d’une irréductible complexité esthétique et discursive</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>Les scènes de bataille rangée dans le cinéma hollywoodien contemporain (1995-2011) : Formatage et renouvellement d’une séquence stratégique</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2011PA100200</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T112" t="inlineStr">
+        <is>
+          <t>La banalisation de la scène de bataille rangée dans le ... se révèlent ainsi porteuses d’une irréductible complexité esthétique et discursive</t>
+        </is>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Yvonne Bourgon-Amir</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Gérard Godron</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ART ET ARCHEOLOGIE</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance en 1988</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Montpellier 3</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Introduction a d'ou viennent ces tissus et qui sont les coptes? b a quoi servaient ces tissus? quelles est leur place dans l'histoire de l'art? d est-il possible de les dater? i scenes 1 le theme imperial, scenes de chasse, combats de gladiateurs, scenes de guerre. 2 scenes bucoliques; 3 scenes bibliques et chretiennes; 4 scenes mythologiques. 5 scenes non identifiees. Ii figures seules, 1 portraits, bustes, masques; 2 figures en pied, vetues; nues. Iii symboles, l'arbre de vie; symboles chretiens, symboles islamiques; et motifs decoratifs, qui furent peut-etre un jour des symboles : motifs sassanides, coupes d'offrandes, "calices de vie", suites de coeurs. Iv animaux allant de l'ours a l'abeille, y compris les animaux fantastiques. V plantes : 1 plantes naturalistes; 2 rinceaux, tiges courbes; 3 rameaux tiges droites; 4 fleurons, fleurs vues de profil; 5 rosaces, fleurs vues de dessus. Vi motifs abstraits, generalement bicolores, entrelacs, meandres; gemmes. Vii le reste : les incomprehensibles; les petits bouts, trop incomplets pour etre etudies.</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>Catalogue thematique des tapisseries coptes du musee historique des tissus de lyon</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>https://theses.fr/1988MON30063</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>Introduction a d'ou viennent ces tissus et qui sont les ... les incomprehensibles; les petits bouts, trop incomplets pour etre etudies.</t>
+        </is>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Hadrien Bru</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Maurice Sartre</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Thèse de doctorat</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Histoire ancienne</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Soutenance en 2005</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Tours</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>L'étude est une mise au point en ce qui concerne le culte impérial au Proche-Orient et ses formes d'expression, en analysant quelles furent la place de l'empereur et de l'image du pouvoir impérial dans le temps et dans l'espace, d'Auguste à Constantin. Les sources épigraphiques, littéraires, numismatiques et archéologiques (sculptures ; architecture monumentale ; urbanisme) sont analysées, de la Phénicie à l'Osrhoène, de la Commagène à l'Arabie. La première partie traite des espaces urbains, ruraux, et des sanctuaires où les représentations figurées et écrites du pouvoir impérial prenaient place, en insistant sur l'ubiquité de " l'empereur géomètre ". La deuxième partie s'intéresse aux fonctions symboliques des représentations sculptées et aux figures religieuses attachées à l'expression d'un pouvoir théoriquement éternel, sans négliger l'approche des épithètes impériales. La troisième partie analyse les célébrations, l'organisation et la promotion du culte impérial : sont abordés les concours grecs, la gladiature, les structures civiques, provinciales et supra-provinciales du culte, avant de conclure par le rôle prépondérant des rois-clients régionaux, des notables civiques et des gouverneurs.</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>Représentations et célébrations du pouvoir impérial dans les provinces syriennes d'Auguste à Constantin : (31 av. J.C.- 337 apr. J.-C.)</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>https://theses.fr/2005TOUR2011</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="T114" t="inlineStr">
+        <is>
+          <t>L'étude est une mise au point en ce qui concerne ... prépondérant des rois-clients régionaux, des notables civiques et des gouverneurs.</t>
+        </is>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>https://theses.fr/resultats?q=gladiator&amp;page=1&amp;nb=100&amp;tri=pertinence&amp;domaine=theses</t>
+        </is>
+      </c>
+      <c r="V114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="W114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
+        </is>
+      </c>
+      <c r="X114" t="inlineStr">
+        <is>
+          <t>Missing value</t>
         </is>
       </c>
     </row>

</xml_diff>